<commit_message>
Added "Names" to Excel Exercise and Checking
</commit_message>
<xml_diff>
--- a/02_Excel/Musterlösung_02.xlsx
+++ b/02_Excel/Musterlösung_02.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacobs/GIT/PC_Praktikum/02_Excel/Excel_Files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacobs/GIT/PC_Praktikum/02_Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{217B88D8-01DF-7242-A762-25506BD24A7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E5F745C-5CDA-AE4C-BE07-9A991477D86A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="2720" windowWidth="30680" windowHeight="26080" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1880" yWindow="2720" windowWidth="30680" windowHeight="26080" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1) Formel" sheetId="1" r:id="rId1"/>
     <sheet name="2) Prüfung" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="Note_Praktikum">'2) Prüfung'!$E$1</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -67,7 +70,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -121,8 +124,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1690,7 +1693,7 @@
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q39" sqref="Q39"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1782,47 +1785,47 @@
         <v>1</v>
       </c>
       <c r="C7" s="5">
-        <f>$B$2*$E$1+$B$3*C$6+$B$4*$B7</f>
+        <f>$B$2*Note_Praktikum+$B$3*C$6+$B$4*$B7</f>
         <v>1.2000000000000002</v>
       </c>
       <c r="D7" s="5">
-        <f t="shared" ref="D7:M7" si="0">$B$2*$E$1+$B$3*D$6+$B$4*$B7</f>
+        <f>$B$2*Note_Praktikum+$B$3*D$6+$B$4*$B7</f>
         <v>1.2600000000000002</v>
       </c>
       <c r="E7" s="5">
-        <f t="shared" si="0"/>
+        <f>$B$2*Note_Praktikum+$B$3*E$6+$B$4*$B7</f>
         <v>1.34</v>
       </c>
       <c r="F7" s="5">
-        <f t="shared" si="0"/>
+        <f>$B$2*Note_Praktikum+$B$3*F$6+$B$4*$B7</f>
         <v>1.4000000000000001</v>
       </c>
       <c r="G7" s="5">
-        <f t="shared" si="0"/>
+        <f>$B$2*Note_Praktikum+$B$3*G$6+$B$4*$B7</f>
         <v>1.46</v>
       </c>
       <c r="H7" s="5">
-        <f t="shared" si="0"/>
+        <f>$B$2*Note_Praktikum+$B$3*H$6+$B$4*$B7</f>
         <v>1.54</v>
       </c>
       <c r="I7" s="5">
-        <f t="shared" si="0"/>
+        <f>$B$2*Note_Praktikum+$B$3*I$6+$B$4*$B7</f>
         <v>1.6</v>
       </c>
       <c r="J7" s="5">
-        <f t="shared" si="0"/>
+        <f>$B$2*Note_Praktikum+$B$3*J$6+$B$4*$B7</f>
         <v>1.6600000000000001</v>
       </c>
       <c r="K7" s="5">
-        <f t="shared" si="0"/>
+        <f>$B$2*Note_Praktikum+$B$3*K$6+$B$4*$B7</f>
         <v>1.7400000000000002</v>
       </c>
       <c r="L7" s="5">
-        <f t="shared" si="0"/>
+        <f>$B$2*Note_Praktikum+$B$3*L$6+$B$4*$B7</f>
         <v>1.8000000000000003</v>
       </c>
       <c r="M7" s="5">
-        <f t="shared" si="0"/>
+        <f>$B$2*Note_Praktikum+$B$3*M$6+$B$4*$B7</f>
         <v>2</v>
       </c>
     </row>
@@ -1831,47 +1834,47 @@
         <v>1.3</v>
       </c>
       <c r="C8" s="5">
-        <f t="shared" ref="C8:M17" si="1">$B$2*$E$1+$B$3*C$6+$B$4*$B8</f>
+        <f>$B$2*Note_Praktikum+$B$3*C$6+$B$4*$B8</f>
         <v>1.3800000000000003</v>
       </c>
       <c r="D8" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*D$6+$B$4*$B8</f>
         <v>1.4400000000000002</v>
       </c>
       <c r="E8" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*E$6+$B$4*$B8</f>
         <v>1.52</v>
       </c>
       <c r="F8" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*F$6+$B$4*$B8</f>
         <v>1.58</v>
       </c>
       <c r="G8" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*G$6+$B$4*$B8</f>
         <v>1.6400000000000001</v>
       </c>
       <c r="H8" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*H$6+$B$4*$B8</f>
         <v>1.7200000000000002</v>
       </c>
       <c r="I8" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*I$6+$B$4*$B8</f>
         <v>1.7800000000000002</v>
       </c>
       <c r="J8" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*J$6+$B$4*$B8</f>
         <v>1.8400000000000003</v>
       </c>
       <c r="K8" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*K$6+$B$4*$B8</f>
         <v>1.9200000000000004</v>
       </c>
       <c r="L8" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*L$6+$B$4*$B8</f>
         <v>1.9800000000000004</v>
       </c>
       <c r="M8" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*M$6+$B$4*$B8</f>
         <v>2.1800000000000002</v>
       </c>
     </row>
@@ -1880,47 +1883,47 @@
         <v>1.7</v>
       </c>
       <c r="C9" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*C$6+$B$4*$B9</f>
         <v>1.62</v>
       </c>
       <c r="D9" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*D$6+$B$4*$B9</f>
         <v>1.6800000000000002</v>
       </c>
       <c r="E9" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*E$6+$B$4*$B9</f>
         <v>1.76</v>
       </c>
       <c r="F9" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*F$6+$B$4*$B9</f>
         <v>1.82</v>
       </c>
       <c r="G9" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*G$6+$B$4*$B9</f>
         <v>1.88</v>
       </c>
       <c r="H9" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*H$6+$B$4*$B9</f>
         <v>1.96</v>
       </c>
       <c r="I9" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*I$6+$B$4*$B9</f>
         <v>2.02</v>
       </c>
       <c r="J9" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*J$6+$B$4*$B9</f>
         <v>2.08</v>
       </c>
       <c r="K9" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*K$6+$B$4*$B9</f>
         <v>2.16</v>
       </c>
       <c r="L9" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*L$6+$B$4*$B9</f>
         <v>2.2200000000000002</v>
       </c>
       <c r="M9" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*M$6+$B$4*$B9</f>
         <v>2.42</v>
       </c>
     </row>
@@ -1929,47 +1932,47 @@
         <v>2</v>
       </c>
       <c r="C10" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*C$6+$B$4*$B10</f>
         <v>1.8000000000000003</v>
       </c>
       <c r="D10" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*D$6+$B$4*$B10</f>
         <v>1.8600000000000003</v>
       </c>
       <c r="E10" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*E$6+$B$4*$B10</f>
         <v>1.9400000000000002</v>
       </c>
       <c r="F10" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*F$6+$B$4*$B10</f>
         <v>2</v>
       </c>
       <c r="G10" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*G$6+$B$4*$B10</f>
         <v>2.06</v>
       </c>
       <c r="H10" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*H$6+$B$4*$B10</f>
         <v>2.14</v>
       </c>
       <c r="I10" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*I$6+$B$4*$B10</f>
         <v>2.2000000000000002</v>
       </c>
       <c r="J10" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*J$6+$B$4*$B10</f>
         <v>2.2600000000000002</v>
       </c>
       <c r="K10" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*K$6+$B$4*$B10</f>
         <v>2.3400000000000003</v>
       </c>
       <c r="L10" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*L$6+$B$4*$B10</f>
         <v>2.4000000000000004</v>
       </c>
       <c r="M10" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*M$6+$B$4*$B10</f>
         <v>2.6</v>
       </c>
     </row>
@@ -1978,47 +1981,47 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="C11" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*C$6+$B$4*$B11</f>
         <v>1.9800000000000002</v>
       </c>
       <c r="D11" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*D$6+$B$4*$B11</f>
         <v>2.04</v>
       </c>
       <c r="E11" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*E$6+$B$4*$B11</f>
         <v>2.12</v>
       </c>
       <c r="F11" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*F$6+$B$4*$B11</f>
         <v>2.1800000000000002</v>
       </c>
       <c r="G11" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*G$6+$B$4*$B11</f>
         <v>2.2400000000000002</v>
       </c>
       <c r="H11" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*H$6+$B$4*$B11</f>
         <v>2.3200000000000003</v>
       </c>
       <c r="I11" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*I$6+$B$4*$B11</f>
         <v>2.38</v>
       </c>
       <c r="J11" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*J$6+$B$4*$B11</f>
         <v>2.4400000000000004</v>
       </c>
       <c r="K11" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*K$6+$B$4*$B11</f>
         <v>2.5200000000000005</v>
       </c>
       <c r="L11" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*L$6+$B$4*$B11</f>
         <v>2.58</v>
       </c>
       <c r="M11" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*M$6+$B$4*$B11</f>
         <v>2.7800000000000002</v>
       </c>
     </row>
@@ -2027,47 +2030,47 @@
         <v>2.7</v>
       </c>
       <c r="C12" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*C$6+$B$4*$B12</f>
         <v>2.2200000000000006</v>
       </c>
       <c r="D12" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*D$6+$B$4*$B12</f>
         <v>2.2800000000000002</v>
       </c>
       <c r="E12" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*E$6+$B$4*$B12</f>
         <v>2.3600000000000003</v>
       </c>
       <c r="F12" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*F$6+$B$4*$B12</f>
         <v>2.4200000000000004</v>
       </c>
       <c r="G12" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*G$6+$B$4*$B12</f>
         <v>2.4800000000000004</v>
       </c>
       <c r="H12" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*H$6+$B$4*$B12</f>
         <v>2.5600000000000005</v>
       </c>
       <c r="I12" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*I$6+$B$4*$B12</f>
         <v>2.62</v>
       </c>
       <c r="J12" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*J$6+$B$4*$B12</f>
         <v>2.6800000000000006</v>
       </c>
       <c r="K12" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*K$6+$B$4*$B12</f>
         <v>2.7600000000000007</v>
       </c>
       <c r="L12" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*L$6+$B$4*$B12</f>
         <v>2.8200000000000003</v>
       </c>
       <c r="M12" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*M$6+$B$4*$B12</f>
         <v>3.0200000000000005</v>
       </c>
     </row>
@@ -2076,47 +2079,47 @@
         <v>3</v>
       </c>
       <c r="C13" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*C$6+$B$4*$B13</f>
         <v>2.4000000000000004</v>
       </c>
       <c r="D13" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*D$6+$B$4*$B13</f>
         <v>2.4600000000000004</v>
       </c>
       <c r="E13" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*E$6+$B$4*$B13</f>
         <v>2.54</v>
       </c>
       <c r="F13" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*F$6+$B$4*$B13</f>
         <v>2.6000000000000005</v>
       </c>
       <c r="G13" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*G$6+$B$4*$B13</f>
         <v>2.66</v>
       </c>
       <c r="H13" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*H$6+$B$4*$B13</f>
         <v>2.74</v>
       </c>
       <c r="I13" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*I$6+$B$4*$B13</f>
         <v>2.8000000000000003</v>
       </c>
       <c r="J13" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*J$6+$B$4*$B13</f>
         <v>2.8600000000000003</v>
       </c>
       <c r="K13" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*K$6+$B$4*$B13</f>
         <v>2.9400000000000004</v>
       </c>
       <c r="L13" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*L$6+$B$4*$B13</f>
         <v>3.0000000000000004</v>
       </c>
       <c r="M13" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*M$6+$B$4*$B13</f>
         <v>3.2</v>
       </c>
     </row>
@@ -2125,47 +2128,47 @@
         <v>3.3</v>
       </c>
       <c r="C14" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*C$6+$B$4*$B14</f>
         <v>2.58</v>
       </c>
       <c r="D14" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*D$6+$B$4*$B14</f>
         <v>2.64</v>
       </c>
       <c r="E14" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*E$6+$B$4*$B14</f>
         <v>2.72</v>
       </c>
       <c r="F14" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*F$6+$B$4*$B14</f>
         <v>2.7800000000000002</v>
       </c>
       <c r="G14" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*G$6+$B$4*$B14</f>
         <v>2.8400000000000003</v>
       </c>
       <c r="H14" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*H$6+$B$4*$B14</f>
         <v>2.9200000000000004</v>
       </c>
       <c r="I14" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*I$6+$B$4*$B14</f>
         <v>2.9800000000000004</v>
       </c>
       <c r="J14" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*J$6+$B$4*$B14</f>
         <v>3.04</v>
       </c>
       <c r="K14" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*K$6+$B$4*$B14</f>
         <v>3.12</v>
       </c>
       <c r="L14" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*L$6+$B$4*$B14</f>
         <v>3.1800000000000006</v>
       </c>
       <c r="M14" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*M$6+$B$4*$B14</f>
         <v>3.38</v>
       </c>
     </row>
@@ -2174,47 +2177,47 @@
         <v>3.7</v>
       </c>
       <c r="C15" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*C$6+$B$4*$B15</f>
         <v>2.8200000000000007</v>
       </c>
       <c r="D15" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*D$6+$B$4*$B15</f>
         <v>2.8800000000000008</v>
       </c>
       <c r="E15" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*E$6+$B$4*$B15</f>
         <v>2.9600000000000009</v>
       </c>
       <c r="F15" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*F$6+$B$4*$B15</f>
         <v>3.0200000000000005</v>
       </c>
       <c r="G15" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*G$6+$B$4*$B15</f>
         <v>3.0800000000000005</v>
       </c>
       <c r="H15" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*H$6+$B$4*$B15</f>
         <v>3.1600000000000006</v>
       </c>
       <c r="I15" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*I$6+$B$4*$B15</f>
         <v>3.2200000000000006</v>
       </c>
       <c r="J15" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*J$6+$B$4*$B15</f>
         <v>3.2800000000000007</v>
       </c>
       <c r="K15" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*K$6+$B$4*$B15</f>
         <v>3.3600000000000008</v>
       </c>
       <c r="L15" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*L$6+$B$4*$B15</f>
         <v>3.4200000000000008</v>
       </c>
       <c r="M15" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*M$6+$B$4*$B15</f>
         <v>3.6200000000000006</v>
       </c>
     </row>
@@ -2223,47 +2226,47 @@
         <v>4</v>
       </c>
       <c r="C16" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*C$6+$B$4*$B16</f>
         <v>3.0000000000000004</v>
       </c>
       <c r="D16" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*D$6+$B$4*$B16</f>
         <v>3.0600000000000005</v>
       </c>
       <c r="E16" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*E$6+$B$4*$B16</f>
         <v>3.1400000000000006</v>
       </c>
       <c r="F16" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*F$6+$B$4*$B16</f>
         <v>3.2</v>
       </c>
       <c r="G16" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*G$6+$B$4*$B16</f>
         <v>3.2600000000000002</v>
       </c>
       <c r="H16" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*H$6+$B$4*$B16</f>
         <v>3.3400000000000003</v>
       </c>
       <c r="I16" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*I$6+$B$4*$B16</f>
         <v>3.4000000000000004</v>
       </c>
       <c r="J16" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*J$6+$B$4*$B16</f>
         <v>3.4600000000000004</v>
       </c>
       <c r="K16" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*K$6+$B$4*$B16</f>
         <v>3.5400000000000005</v>
       </c>
       <c r="L16" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*L$6+$B$4*$B16</f>
         <v>3.6000000000000005</v>
       </c>
       <c r="M16" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*M$6+$B$4*$B16</f>
         <v>3.8000000000000003</v>
       </c>
     </row>
@@ -2272,47 +2275,47 @@
         <v>5</v>
       </c>
       <c r="C17" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*C$6+$B$4*$B17</f>
         <v>3.6000000000000005</v>
       </c>
       <c r="D17" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*D$6+$B$4*$B17</f>
         <v>3.6600000000000006</v>
       </c>
       <c r="E17" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*E$6+$B$4*$B17</f>
         <v>3.74</v>
       </c>
       <c r="F17" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*F$6+$B$4*$B17</f>
         <v>3.8000000000000007</v>
       </c>
       <c r="G17" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*G$6+$B$4*$B17</f>
         <v>3.8600000000000003</v>
       </c>
       <c r="H17" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*H$6+$B$4*$B17</f>
         <v>3.9400000000000004</v>
       </c>
       <c r="I17" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*I$6+$B$4*$B17</f>
         <v>4</v>
       </c>
       <c r="J17" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*J$6+$B$4*$B17</f>
         <v>4.0600000000000005</v>
       </c>
       <c r="K17" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*K$6+$B$4*$B17</f>
         <v>4.1400000000000006</v>
       </c>
       <c r="L17" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*L$6+$B$4*$B17</f>
         <v>4.2000000000000011</v>
       </c>
       <c r="M17" s="5">
-        <f t="shared" si="1"/>
+        <f>$B$2*Note_Praktikum+$B$3*M$6+$B$4*$B17</f>
         <v>4.4000000000000004</v>
       </c>
     </row>

</xml_diff>